<commit_message>
Update before sharing with Maria
</commit_message>
<xml_diff>
--- a/simmod/partitioning/parametric senescence.xlsx
+++ b/simmod/partitioning/parametric senescence.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -139,7 +139,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -386,6 +386,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D629-4D04-AB76-4CD4C8C8FA3D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -624,6 +629,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D629-4D04-AB76-4CD4C8C8FA3D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -691,7 +701,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2120607712"/>
@@ -753,7 +763,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2120620768"/>
@@ -796,7 +806,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -826,7 +836,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -838,7 +848,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1094,6 +1104,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4F36-4A35-ACA2-A168DA4DEE23}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1161,7 +1176,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2120612064"/>
@@ -1223,7 +1238,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2120610976"/>
@@ -1266,7 +1281,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1296,7 +1311,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2776,7 +2791,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>